<commit_message>
Added fixed and results
</commit_message>
<xml_diff>
--- a/code/results_cells/results_cec2017_10.xlsx
+++ b/code/results_cells/results_cec2017_10.xlsx
@@ -579,94 +579,94 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2652250000</v>
+        <v>4387022300</v>
       </c>
       <c r="D2">
-        <v>4036976380</v>
+        <v>38517983246</v>
       </c>
       <c r="E2">
-        <v>22635.085</v>
+        <v>22259.859</v>
       </c>
       <c r="F2">
-        <v>204.500565</v>
+        <v>316.58956</v>
       </c>
       <c r="G2">
-        <v>68.73413299999999</v>
+        <v>81.182012</v>
       </c>
       <c r="H2">
-        <v>31.498818</v>
+        <v>41.13112300000001</v>
       </c>
       <c r="I2">
-        <v>136.432591</v>
+        <v>158.47065</v>
       </c>
       <c r="J2">
-        <v>71.24881000000001</v>
+        <v>75.068162</v>
       </c>
       <c r="K2">
-        <v>752.3324</v>
+        <v>1116.15303</v>
       </c>
       <c r="L2">
-        <v>1617.8389</v>
+        <v>1690.385</v>
       </c>
       <c r="M2">
-        <v>683.1988700000001</v>
+        <v>1267.38116</v>
       </c>
       <c r="N2">
-        <v>127233112</v>
+        <v>187925056</v>
       </c>
       <c r="O2">
-        <v>15232266.5</v>
+        <v>10607031.28</v>
       </c>
       <c r="P2">
-        <v>29922.58014</v>
+        <v>40077.06665</v>
       </c>
       <c r="Q2">
-        <v>100727.6638</v>
+        <v>147615.7086</v>
       </c>
       <c r="R2">
-        <v>503.75618</v>
+        <v>516.3798899999999</v>
       </c>
       <c r="S2">
-        <v>217.2098</v>
+        <v>271.36357</v>
       </c>
       <c r="T2">
-        <v>20955671.9</v>
+        <v>27540926.2</v>
       </c>
       <c r="U2">
-        <v>949877.324</v>
+        <v>652213.0730000001</v>
       </c>
       <c r="V2">
-        <v>261.32536</v>
+        <v>264.02026</v>
       </c>
       <c r="W2">
-        <v>216.29218</v>
+        <v>252.24142</v>
       </c>
       <c r="X2">
-        <v>385.2876199999999</v>
+        <v>439.1586900000001</v>
       </c>
       <c r="Y2">
-        <v>385.00342</v>
+        <v>402.4726899999999</v>
       </c>
       <c r="Z2">
-        <v>396.86793</v>
+        <v>399.67708</v>
       </c>
       <c r="AA2">
-        <v>618.3262400000001</v>
+        <v>705.1403200000001</v>
       </c>
       <c r="AB2">
-        <v>913.1301899999999</v>
+        <v>1161.3235</v>
       </c>
       <c r="AC2">
-        <v>456.62255</v>
+        <v>485.4586700000001</v>
       </c>
       <c r="AD2">
-        <v>823.9554700000002</v>
+        <v>932.77212</v>
       </c>
       <c r="AE2">
-        <v>456.9112899999999</v>
+        <v>518.1744600000001</v>
       </c>
       <c r="AF2">
-        <v>8983533</v>
+        <v>14538764.7</v>
       </c>
       <c r="AG2">
         <v>10</v>
@@ -680,94 +680,94 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>2283645000</v>
+        <v>3612538200</v>
       </c>
       <c r="D3">
-        <v>1888558636</v>
+        <v>7969395036</v>
       </c>
       <c r="E3">
-        <v>18757.325</v>
+        <v>20405.695</v>
       </c>
       <c r="F3">
-        <v>153.905694</v>
+        <v>284.05587</v>
       </c>
       <c r="G3">
-        <v>64.517031</v>
+        <v>78.049769</v>
       </c>
       <c r="H3">
-        <v>27.680935</v>
+        <v>40.626605</v>
       </c>
       <c r="I3">
-        <v>119.817071</v>
+        <v>158.47065</v>
       </c>
       <c r="J3">
-        <v>60.529006</v>
+        <v>69.577079</v>
       </c>
       <c r="K3">
-        <v>639.67337</v>
+        <v>1060.51493</v>
       </c>
       <c r="L3">
-        <v>1468.8053</v>
+        <v>1616.4451</v>
       </c>
       <c r="M3">
-        <v>510.2119399999999</v>
+        <v>838.9569000000001</v>
       </c>
       <c r="N3">
-        <v>70098601</v>
+        <v>144668222</v>
       </c>
       <c r="O3">
-        <v>9293966.1</v>
+        <v>6256315.48</v>
       </c>
       <c r="P3">
-        <v>17731.06224</v>
+        <v>19089.52345</v>
       </c>
       <c r="Q3">
-        <v>97534.5845</v>
+        <v>44141.44999</v>
       </c>
       <c r="R3">
-        <v>440.6334199999999</v>
+        <v>446.9368900000001</v>
       </c>
       <c r="S3">
-        <v>179.86652</v>
+        <v>220.73509</v>
       </c>
       <c r="T3">
-        <v>11513771.5</v>
+        <v>13312247.2</v>
       </c>
       <c r="U3">
-        <v>555861.0429999999</v>
+        <v>285460.116</v>
       </c>
       <c r="V3">
-        <v>203.45207</v>
+        <v>246.34255</v>
       </c>
       <c r="W3">
-        <v>187.5197</v>
+        <v>242.37006</v>
       </c>
       <c r="X3">
-        <v>280.21023</v>
+        <v>399.59941</v>
       </c>
       <c r="Y3">
-        <v>374.23247</v>
+        <v>396.22745</v>
       </c>
       <c r="Z3">
-        <v>376.61731</v>
+        <v>374.43624</v>
       </c>
       <c r="AA3">
-        <v>570.7226700000001</v>
+        <v>688.1389400000002</v>
       </c>
       <c r="AB3">
-        <v>851.1192699999999</v>
+        <v>1080.59246</v>
       </c>
       <c r="AC3">
-        <v>440.6378099999999</v>
+        <v>475.86788</v>
       </c>
       <c r="AD3">
-        <v>732.41811</v>
+        <v>866.14725</v>
       </c>
       <c r="AE3">
-        <v>434.26014</v>
+        <v>503.8591300000001</v>
       </c>
       <c r="AF3">
-        <v>4667084.4</v>
+        <v>8133094.609999999</v>
       </c>
       <c r="AG3">
         <v>10</v>
@@ -781,94 +781,94 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>1823825400</v>
+        <v>3612538200</v>
       </c>
       <c r="D4">
-        <v>324538759</v>
+        <v>7969395036</v>
       </c>
       <c r="E4">
-        <v>17308.051</v>
+        <v>17322.295</v>
       </c>
       <c r="F4">
-        <v>119.941804</v>
+        <v>284.05587</v>
       </c>
       <c r="G4">
-        <v>58.26143399999999</v>
+        <v>77.675398</v>
       </c>
       <c r="H4">
-        <v>25.704627</v>
+        <v>40.626605</v>
       </c>
       <c r="I4">
-        <v>111.398617</v>
+        <v>157.21382</v>
       </c>
       <c r="J4">
-        <v>56.06273700000001</v>
+        <v>69.577079</v>
       </c>
       <c r="K4">
-        <v>591.1161500000001</v>
+        <v>1010.23663</v>
       </c>
       <c r="L4">
-        <v>1400.3701</v>
+        <v>1598.2555</v>
       </c>
       <c r="M4">
-        <v>311.32895</v>
+        <v>838.9569000000001</v>
       </c>
       <c r="N4">
-        <v>49132578</v>
+        <v>123510952</v>
       </c>
       <c r="O4">
-        <v>4679209.939999999</v>
+        <v>1905869.65</v>
       </c>
       <c r="P4">
-        <v>8064.553740000001</v>
+        <v>5086.32965</v>
       </c>
       <c r="Q4">
-        <v>26491.44609999999</v>
+        <v>9686.132589999999</v>
       </c>
       <c r="R4">
-        <v>409.29042</v>
+        <v>443.9163</v>
       </c>
       <c r="S4">
-        <v>150.604034</v>
+        <v>198.62449</v>
       </c>
       <c r="T4">
-        <v>8081131.3</v>
+        <v>11607506.17</v>
       </c>
       <c r="U4">
-        <v>308553.1866</v>
+        <v>202397.5592</v>
       </c>
       <c r="V4">
-        <v>175.55586</v>
+        <v>230.73033</v>
       </c>
       <c r="W4">
-        <v>184.14287</v>
+        <v>211.60134</v>
       </c>
       <c r="X4">
-        <v>248.38291</v>
+        <v>399.59941</v>
       </c>
       <c r="Y4">
-        <v>371.55587</v>
+        <v>396.22745</v>
       </c>
       <c r="Z4">
-        <v>359.33713</v>
+        <v>374.43624</v>
       </c>
       <c r="AA4">
-        <v>539.98884</v>
+        <v>672.2821700000001</v>
       </c>
       <c r="AB4">
-        <v>727.3227000000001</v>
+        <v>1070.76976</v>
       </c>
       <c r="AC4">
-        <v>436.4422699999999</v>
+        <v>472.62535</v>
       </c>
       <c r="AD4">
-        <v>707.7053</v>
+        <v>839.1653700000001</v>
       </c>
       <c r="AE4">
-        <v>402.7851699999999</v>
+        <v>488.68951</v>
       </c>
       <c r="AF4">
-        <v>3715345.7</v>
+        <v>6976029.709999999</v>
       </c>
       <c r="AG4">
         <v>10</v>
@@ -882,94 +882,94 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>1414953480</v>
+        <v>3237532700</v>
       </c>
       <c r="D5">
-        <v>184610135.1</v>
+        <v>4665804481</v>
       </c>
       <c r="E5">
-        <v>15043.3105</v>
+        <v>15674.923</v>
       </c>
       <c r="F5">
-        <v>103.099111</v>
+        <v>271.449009</v>
       </c>
       <c r="G5">
-        <v>54.070559</v>
+        <v>76.238967</v>
       </c>
       <c r="H5">
-        <v>22.965087</v>
+        <v>40.460216</v>
       </c>
       <c r="I5">
-        <v>101.752883</v>
+        <v>151.92725</v>
       </c>
       <c r="J5">
-        <v>52.12306099999999</v>
+        <v>67.96695000000001</v>
       </c>
       <c r="K5">
-        <v>490.1387199999999</v>
+        <v>1003.73083</v>
       </c>
       <c r="L5">
-        <v>1391.1595</v>
+        <v>1564.6829</v>
       </c>
       <c r="M5">
-        <v>280.54754</v>
+        <v>801.56593</v>
       </c>
       <c r="N5">
-        <v>40137003</v>
+        <v>94070879</v>
       </c>
       <c r="O5">
-        <v>2364356.96</v>
+        <v>1075438.62</v>
       </c>
       <c r="P5">
-        <v>7146.451770000001</v>
+        <v>4292.02137</v>
       </c>
       <c r="Q5">
-        <v>24596.4727</v>
+        <v>7315.711690000001</v>
       </c>
       <c r="R5">
-        <v>296.05206</v>
+        <v>424.4263</v>
       </c>
       <c r="S5">
-        <v>120.038852</v>
+        <v>181.69563</v>
       </c>
       <c r="T5">
-        <v>6834498.1</v>
+        <v>5704452.970000001</v>
       </c>
       <c r="U5">
-        <v>179258.4035</v>
+        <v>76953.3392</v>
       </c>
       <c r="V5">
-        <v>162.45777</v>
+        <v>213.57194</v>
       </c>
       <c r="W5">
-        <v>167.37556</v>
+        <v>184.20233</v>
       </c>
       <c r="X5">
-        <v>230.7863</v>
+        <v>365.74446</v>
       </c>
       <c r="Y5">
-        <v>367.07502</v>
+        <v>391.72706</v>
       </c>
       <c r="Z5">
-        <v>325.1086900000001</v>
+        <v>370.71843</v>
       </c>
       <c r="AA5">
-        <v>523.9925799999999</v>
+        <v>627.8248000000001</v>
       </c>
       <c r="AB5">
-        <v>683.4912800000001</v>
+        <v>979.2091</v>
       </c>
       <c r="AC5">
-        <v>429.06816</v>
+        <v>462.72698</v>
       </c>
       <c r="AD5">
-        <v>652.60574</v>
+        <v>784.91034</v>
       </c>
       <c r="AE5">
-        <v>389.18068</v>
+        <v>467.6623500000001</v>
       </c>
       <c r="AF5">
-        <v>3392118.4</v>
+        <v>6687329.71</v>
       </c>
       <c r="AG5">
         <v>10</v>
@@ -983,94 +983,94 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>992887020</v>
+        <v>3237532700</v>
       </c>
       <c r="D6">
-        <v>60564522.2</v>
+        <v>2240219881</v>
       </c>
       <c r="E6">
-        <v>12621.962</v>
+        <v>14623.567</v>
       </c>
       <c r="F6">
-        <v>73.731255</v>
+        <v>251.266069</v>
       </c>
       <c r="G6">
-        <v>46.982985</v>
+        <v>74.25761600000001</v>
       </c>
       <c r="H6">
-        <v>20.519138</v>
+        <v>40.218206</v>
       </c>
       <c r="I6">
-        <v>91.32149</v>
+        <v>151.92725</v>
       </c>
       <c r="J6">
-        <v>48.449408</v>
+        <v>66.898565</v>
       </c>
       <c r="K6">
-        <v>361.66832</v>
+        <v>903.4169599999999</v>
       </c>
       <c r="L6">
-        <v>1290.3539</v>
+        <v>1553.2638</v>
       </c>
       <c r="M6">
-        <v>207.541109</v>
+        <v>670.6767599999999</v>
       </c>
       <c r="N6">
-        <v>31164397.8</v>
+        <v>93960189</v>
       </c>
       <c r="O6">
-        <v>811756.4999999999</v>
+        <v>749301.8</v>
       </c>
       <c r="P6">
-        <v>3162.86937</v>
+        <v>2571.11078</v>
       </c>
       <c r="Q6">
-        <v>6771.5705</v>
+        <v>7253.805390000001</v>
       </c>
       <c r="R6">
-        <v>228.916104</v>
+        <v>388.41274</v>
       </c>
       <c r="S6">
-        <v>106.696028</v>
+        <v>162.83807</v>
       </c>
       <c r="T6">
-        <v>1319164.4092</v>
+        <v>2703574.24</v>
       </c>
       <c r="U6">
-        <v>15043.7073</v>
+        <v>18759.6506</v>
       </c>
       <c r="V6">
-        <v>129.032976</v>
+        <v>180.99624</v>
       </c>
       <c r="W6">
-        <v>151.70214</v>
+        <v>172.8804</v>
       </c>
       <c r="X6">
-        <v>194.78148</v>
+        <v>318.46705</v>
       </c>
       <c r="Y6">
-        <v>363.76775</v>
+        <v>391.72706</v>
       </c>
       <c r="Z6">
-        <v>311.84542</v>
+        <v>346.39027</v>
       </c>
       <c r="AA6">
-        <v>505.7022700000001</v>
+        <v>600.56883</v>
       </c>
       <c r="AB6">
-        <v>645.0507900000001</v>
+        <v>915.0736600000002</v>
       </c>
       <c r="AC6">
-        <v>421.953</v>
+        <v>456.84014</v>
       </c>
       <c r="AD6">
-        <v>579.73906</v>
+        <v>748.2246</v>
       </c>
       <c r="AE6">
-        <v>371.04408</v>
+        <v>457.38607</v>
       </c>
       <c r="AF6">
-        <v>2144142.933</v>
+        <v>5126553.71</v>
       </c>
       <c r="AG6">
         <v>10</v>
@@ -1084,94 +1084,94 @@
         <v>20</v>
       </c>
       <c r="C7">
-        <v>754829370</v>
+        <v>3179003000</v>
       </c>
       <c r="D7">
-        <v>30172623.2</v>
+        <v>734900234</v>
       </c>
       <c r="E7">
-        <v>11274.3199</v>
+        <v>12029.9381</v>
       </c>
       <c r="F7">
-        <v>60.840428</v>
+        <v>231.565019</v>
       </c>
       <c r="G7">
-        <v>43.598168</v>
+        <v>73.784486</v>
       </c>
       <c r="H7">
-        <v>19.619409</v>
+        <v>37.805939</v>
       </c>
       <c r="I7">
-        <v>84.970448</v>
+        <v>148.00119</v>
       </c>
       <c r="J7">
-        <v>44.482304</v>
+        <v>61.966575</v>
       </c>
       <c r="K7">
-        <v>339.16837</v>
+        <v>862.3809799999999</v>
       </c>
       <c r="L7">
-        <v>1211.4336</v>
+        <v>1465.4558</v>
       </c>
       <c r="M7">
-        <v>155.977197</v>
+        <v>570.0847200000001</v>
       </c>
       <c r="N7">
-        <v>22770216</v>
+        <v>77701957</v>
       </c>
       <c r="O7">
-        <v>390082.64</v>
+        <v>308477.1690000001</v>
       </c>
       <c r="P7">
-        <v>1777.80562</v>
+        <v>1134.06733</v>
       </c>
       <c r="Q7">
-        <v>2946.4052</v>
+        <v>3367.99009</v>
       </c>
       <c r="R7">
-        <v>213.488564</v>
+        <v>332.54642</v>
       </c>
       <c r="S7">
-        <v>93.32810299999998</v>
+        <v>154.74628</v>
       </c>
       <c r="T7">
-        <v>621364.7946</v>
+        <v>1385773.27</v>
       </c>
       <c r="U7">
-        <v>5982.87746</v>
+        <v>7288.4072</v>
       </c>
       <c r="V7">
-        <v>108.402724</v>
+        <v>159.81523</v>
       </c>
       <c r="W7">
-        <v>131.909189</v>
+        <v>164.82731</v>
       </c>
       <c r="X7">
-        <v>171.4268</v>
+        <v>296.50957</v>
       </c>
       <c r="Y7">
-        <v>357.28124</v>
+        <v>387.30288</v>
       </c>
       <c r="Z7">
-        <v>267.39438</v>
+        <v>325.79677</v>
       </c>
       <c r="AA7">
-        <v>494.6094300000001</v>
+        <v>593.4741700000001</v>
       </c>
       <c r="AB7">
-        <v>588.08392</v>
+        <v>794.90372</v>
       </c>
       <c r="AC7">
-        <v>419.07106</v>
+        <v>454.5532800000001</v>
       </c>
       <c r="AD7">
-        <v>530.30055</v>
+        <v>659.94937</v>
       </c>
       <c r="AE7">
-        <v>358.69197</v>
+        <v>431.8470899999999</v>
       </c>
       <c r="AF7">
-        <v>959822.9030000002</v>
+        <v>4933391.41</v>
       </c>
       <c r="AG7">
         <v>10</v>
@@ -1185,94 +1185,94 @@
         <v>30</v>
       </c>
       <c r="C8">
-        <v>552307970</v>
+        <v>3179003000</v>
       </c>
       <c r="D8">
-        <v>18908242.5</v>
+        <v>679344834</v>
       </c>
       <c r="E8">
-        <v>10061.9716</v>
+        <v>10066.3851</v>
       </c>
       <c r="F8">
-        <v>58.512666</v>
+        <v>208.402629</v>
       </c>
       <c r="G8">
-        <v>41.661967</v>
+        <v>73.56108300000001</v>
       </c>
       <c r="H8">
-        <v>18.428293</v>
+        <v>35.302253</v>
       </c>
       <c r="I8">
-        <v>84.371674</v>
+        <v>148.00119</v>
       </c>
       <c r="J8">
-        <v>44.257685</v>
+        <v>58.89686</v>
       </c>
       <c r="K8">
-        <v>265.66863</v>
+        <v>811.8059099999999</v>
       </c>
       <c r="L8">
-        <v>1103.64258</v>
+        <v>1440.0068</v>
       </c>
       <c r="M8">
-        <v>153.323137</v>
+        <v>424.28271</v>
       </c>
       <c r="N8">
-        <v>17660708</v>
+        <v>70576439</v>
       </c>
       <c r="O8">
-        <v>317604.388</v>
+        <v>161450.542</v>
       </c>
       <c r="P8">
-        <v>1225.29205</v>
+        <v>795.0750599999999</v>
       </c>
       <c r="Q8">
-        <v>2183.59077</v>
+        <v>2743.35269</v>
       </c>
       <c r="R8">
-        <v>172.888869</v>
+        <v>325.9508500000001</v>
       </c>
       <c r="S8">
-        <v>74.074392</v>
+        <v>148.26813</v>
       </c>
       <c r="T8">
-        <v>333862.5316</v>
+        <v>969704.22</v>
       </c>
       <c r="U8">
-        <v>3980.38603</v>
+        <v>5939.631800000001</v>
       </c>
       <c r="V8">
-        <v>101.049063</v>
+        <v>142.79639</v>
       </c>
       <c r="W8">
-        <v>131.909189</v>
+        <v>161.21071</v>
       </c>
       <c r="X8">
-        <v>161.31819</v>
+        <v>273.09499</v>
       </c>
       <c r="Y8">
-        <v>355.3478200000001</v>
+        <v>386.60246</v>
       </c>
       <c r="Z8">
-        <v>263.2698099999999</v>
+        <v>321.77302</v>
       </c>
       <c r="AA8">
-        <v>484.90455</v>
+        <v>581.44803</v>
       </c>
       <c r="AB8">
-        <v>577.1104800000001</v>
+        <v>770.89544</v>
       </c>
       <c r="AC8">
-        <v>418.7145899999999</v>
+        <v>451.71161</v>
       </c>
       <c r="AD8">
-        <v>512.78502</v>
+        <v>646.8042899999999</v>
       </c>
       <c r="AE8">
-        <v>346.49654</v>
+        <v>424.59996</v>
       </c>
       <c r="AF8">
-        <v>856827.6129999999</v>
+        <v>4410262.41</v>
       </c>
       <c r="AG8">
         <v>10</v>
@@ -1286,94 +1286,94 @@
         <v>40</v>
       </c>
       <c r="C9">
-        <v>512380000</v>
+        <v>3081003000</v>
       </c>
       <c r="D9">
-        <v>6172462.7</v>
+        <v>679344834</v>
       </c>
       <c r="E9">
-        <v>9357.634599999999</v>
+        <v>8976.839600000001</v>
       </c>
       <c r="F9">
-        <v>56.660627</v>
+        <v>198.588199</v>
       </c>
       <c r="G9">
-        <v>40.656437</v>
+        <v>71.60204200000001</v>
       </c>
       <c r="H9">
-        <v>17.967238</v>
+        <v>35.302253</v>
       </c>
       <c r="I9">
-        <v>83.74105499999999</v>
+        <v>146.5175</v>
       </c>
       <c r="J9">
-        <v>41.39228799999999</v>
+        <v>58.89686</v>
       </c>
       <c r="K9">
-        <v>265.66863</v>
+        <v>811.8059099999999</v>
       </c>
       <c r="L9">
-        <v>1102.41118</v>
+        <v>1431.7985</v>
       </c>
       <c r="M9">
-        <v>124.277917</v>
+        <v>412.8217</v>
       </c>
       <c r="N9">
-        <v>14708366</v>
+        <v>53909843</v>
       </c>
       <c r="O9">
-        <v>299380.268</v>
+        <v>113117.355</v>
       </c>
       <c r="P9">
-        <v>1081.37255</v>
+        <v>654.904543</v>
       </c>
       <c r="Q9">
-        <v>1825.23858</v>
+        <v>2743.35269</v>
       </c>
       <c r="R9">
-        <v>163.606679</v>
+        <v>325.9508500000001</v>
       </c>
       <c r="S9">
-        <v>71.657293</v>
+        <v>138.87621</v>
       </c>
       <c r="T9">
-        <v>294013.4296</v>
+        <v>887266.6399999999</v>
       </c>
       <c r="U9">
-        <v>3060.35693</v>
+        <v>5825.340750000001</v>
       </c>
       <c r="V9">
-        <v>97.90186500000002</v>
+        <v>138.9101</v>
       </c>
       <c r="W9">
-        <v>129.434779</v>
+        <v>158.02412</v>
       </c>
       <c r="X9">
-        <v>156.26362</v>
+        <v>271.84865</v>
       </c>
       <c r="Y9">
-        <v>351.8076600000001</v>
+        <v>382.8404400000001</v>
       </c>
       <c r="Z9">
-        <v>250.48754</v>
+        <v>306.9401300000001</v>
       </c>
       <c r="AA9">
-        <v>483.5322199999999</v>
+        <v>581.1570800000001</v>
       </c>
       <c r="AB9">
-        <v>567.7444400000001</v>
+        <v>713.94483</v>
       </c>
       <c r="AC9">
-        <v>418.2982899999999</v>
+        <v>450.66618</v>
       </c>
       <c r="AD9">
-        <v>512.27518</v>
+        <v>636.21633</v>
       </c>
       <c r="AE9">
-        <v>338.67233</v>
+        <v>419.78125</v>
       </c>
       <c r="AF9">
-        <v>512971.083</v>
+        <v>4249938.51</v>
       </c>
       <c r="AG9">
         <v>10</v>
@@ -1387,94 +1387,94 @@
         <v>50</v>
       </c>
       <c r="C10">
-        <v>433313980</v>
+        <v>2842217100</v>
       </c>
       <c r="D10">
-        <v>4226827.63</v>
+        <v>560968365</v>
       </c>
       <c r="E10">
-        <v>8252.711399999998</v>
+        <v>8976.839600000001</v>
       </c>
       <c r="F10">
-        <v>56.660627</v>
+        <v>198.588199</v>
       </c>
       <c r="G10">
-        <v>39.154144</v>
+        <v>70.43380099999999</v>
       </c>
       <c r="H10">
-        <v>17.015001</v>
+        <v>34.835567</v>
       </c>
       <c r="I10">
-        <v>80.423967</v>
+        <v>146.5175</v>
       </c>
       <c r="J10">
-        <v>41.167252</v>
+        <v>58.67597600000001</v>
       </c>
       <c r="K10">
-        <v>260.33191</v>
+        <v>806.1688099999999</v>
       </c>
       <c r="L10">
-        <v>1090.74348</v>
+        <v>1418.5967</v>
       </c>
       <c r="M10">
-        <v>99.92612899999999</v>
+        <v>355.32489</v>
       </c>
       <c r="N10">
-        <v>13027890.9</v>
+        <v>51714304</v>
       </c>
       <c r="O10">
-        <v>243873.8480000001</v>
+        <v>113117.355</v>
       </c>
       <c r="P10">
-        <v>843.3008</v>
+        <v>409.636963</v>
       </c>
       <c r="Q10">
-        <v>1690.46388</v>
+        <v>2144.04109</v>
       </c>
       <c r="R10">
-        <v>159.546369</v>
+        <v>290.84221</v>
       </c>
       <c r="S10">
-        <v>65.53521500000001</v>
+        <v>126.85268</v>
       </c>
       <c r="T10">
-        <v>212890.6526</v>
+        <v>795640.84</v>
       </c>
       <c r="U10">
-        <v>2575.22516</v>
+        <v>4691.423650000001</v>
       </c>
       <c r="V10">
-        <v>91.61754000000001</v>
+        <v>131.6402</v>
       </c>
       <c r="W10">
-        <v>128.379949</v>
+        <v>154.03012</v>
       </c>
       <c r="X10">
-        <v>150.74613</v>
+        <v>271.84865</v>
       </c>
       <c r="Y10">
-        <v>350.00027</v>
+        <v>382.8404400000001</v>
       </c>
       <c r="Z10">
-        <v>250.48754</v>
+        <v>306.00122</v>
       </c>
       <c r="AA10">
-        <v>476.40796</v>
+        <v>572.27586</v>
       </c>
       <c r="AB10">
-        <v>549.45796</v>
+        <v>707.9568300000001</v>
       </c>
       <c r="AC10">
-        <v>416.8478699999999</v>
+        <v>448.62503</v>
       </c>
       <c r="AD10">
-        <v>499.5844</v>
+        <v>627.35375</v>
       </c>
       <c r="AE10">
-        <v>328.19965</v>
+        <v>417.93322</v>
       </c>
       <c r="AF10">
-        <v>476573.753</v>
+        <v>3917509.51</v>
       </c>
       <c r="AG10">
         <v>10</v>
@@ -1488,94 +1488,94 @@
         <v>60</v>
       </c>
       <c r="C11">
-        <v>412689420</v>
+        <v>2842217100</v>
       </c>
       <c r="D11">
-        <v>3081696.63</v>
+        <v>476236500</v>
       </c>
       <c r="E11">
-        <v>8046.470699999998</v>
+        <v>8976.839600000001</v>
       </c>
       <c r="F11">
-        <v>51.475491</v>
+        <v>191.888039</v>
       </c>
       <c r="G11">
-        <v>37.609236</v>
+        <v>70.00321299999999</v>
       </c>
       <c r="H11">
-        <v>16.664195</v>
+        <v>33.849969</v>
       </c>
       <c r="I11">
-        <v>78.348572</v>
+        <v>144.11664</v>
       </c>
       <c r="J11">
-        <v>40.055874</v>
+        <v>58.519799</v>
       </c>
       <c r="K11">
-        <v>251.25874</v>
+        <v>796.87203</v>
       </c>
       <c r="L11">
-        <v>1090.74348</v>
+        <v>1414.3756</v>
       </c>
       <c r="M11">
-        <v>99.92612899999999</v>
+        <v>338.89942</v>
       </c>
       <c r="N11">
-        <v>11931002.9</v>
+        <v>51451090</v>
       </c>
       <c r="O11">
-        <v>184114.656</v>
+        <v>106646.225</v>
       </c>
       <c r="P11">
-        <v>747.9889900000001</v>
+        <v>353.9969130000001</v>
       </c>
       <c r="Q11">
-        <v>1690.46388</v>
+        <v>2015.04004</v>
       </c>
       <c r="R11">
-        <v>156.822899</v>
+        <v>290.6131600000001</v>
       </c>
       <c r="S11">
-        <v>64.744027</v>
+        <v>125.70063</v>
       </c>
       <c r="T11">
-        <v>193176.4226</v>
+        <v>597946.41</v>
       </c>
       <c r="U11">
-        <v>2422.96544</v>
+        <v>4234.41038</v>
       </c>
       <c r="V11">
-        <v>83.445284</v>
+        <v>126.8845</v>
       </c>
       <c r="W11">
-        <v>124.264169</v>
+        <v>143.45904</v>
       </c>
       <c r="X11">
-        <v>144.45772</v>
+        <v>268.62043</v>
       </c>
       <c r="Y11">
-        <v>348.82262</v>
+        <v>381.2996</v>
       </c>
       <c r="Z11">
-        <v>248.3069</v>
+        <v>298.59596</v>
       </c>
       <c r="AA11">
-        <v>474.77453</v>
+        <v>572.27586</v>
       </c>
       <c r="AB11">
-        <v>544.1953599999999</v>
+        <v>704.5923700000001</v>
       </c>
       <c r="AC11">
-        <v>415.97526</v>
+        <v>445.5323099999999</v>
       </c>
       <c r="AD11">
-        <v>473.52023</v>
+        <v>620.2553599999999</v>
       </c>
       <c r="AE11">
-        <v>325.75954</v>
+        <v>403.60729</v>
       </c>
       <c r="AF11">
-        <v>432876.743</v>
+        <v>3745339.21</v>
       </c>
       <c r="AG11">
         <v>10</v>
@@ -1589,94 +1589,94 @@
         <v>70</v>
       </c>
       <c r="C12">
-        <v>412689420</v>
+        <v>2733082600</v>
       </c>
       <c r="D12">
-        <v>3081696.63</v>
+        <v>379628800</v>
       </c>
       <c r="E12">
-        <v>7933.077599999999</v>
+        <v>8852.1857</v>
       </c>
       <c r="F12">
-        <v>50.22344099999999</v>
+        <v>179.066669</v>
       </c>
       <c r="G12">
-        <v>37.609236</v>
+        <v>68.853318</v>
       </c>
       <c r="H12">
-        <v>16.565415</v>
+        <v>32.963964</v>
       </c>
       <c r="I12">
-        <v>78.22327600000001</v>
+        <v>144.11664</v>
       </c>
       <c r="J12">
-        <v>39.21806099999999</v>
+        <v>58.519799</v>
       </c>
       <c r="K12">
-        <v>226.2112</v>
+        <v>769.81391</v>
       </c>
       <c r="L12">
-        <v>1053.27963</v>
+        <v>1407.9962</v>
       </c>
       <c r="M12">
-        <v>99.92612899999999</v>
+        <v>338.89942</v>
       </c>
       <c r="N12">
-        <v>10927982.9</v>
+        <v>46652465</v>
       </c>
       <c r="O12">
-        <v>183473.453</v>
+        <v>104581.154</v>
       </c>
       <c r="P12">
-        <v>740.94109</v>
+        <v>330.900523</v>
       </c>
       <c r="Q12">
-        <v>1690.46388</v>
+        <v>2015.04004</v>
       </c>
       <c r="R12">
-        <v>144.991439</v>
+        <v>272.69024</v>
       </c>
       <c r="S12">
-        <v>62.25149700000001</v>
+        <v>120.343948</v>
       </c>
       <c r="T12">
-        <v>170429.1026</v>
+        <v>585116.48</v>
       </c>
       <c r="U12">
-        <v>2422.96544</v>
+        <v>3374.502179999999</v>
       </c>
       <c r="V12">
-        <v>83.445284</v>
+        <v>123.59372</v>
       </c>
       <c r="W12">
-        <v>124.064569</v>
+        <v>139.75586</v>
       </c>
       <c r="X12">
-        <v>144.07482</v>
+        <v>253.0676</v>
       </c>
       <c r="Y12">
-        <v>348.82262</v>
+        <v>379.31119</v>
       </c>
       <c r="Z12">
-        <v>246.38899</v>
+        <v>298.59596</v>
       </c>
       <c r="AA12">
-        <v>465.58164</v>
+        <v>568.89424</v>
       </c>
       <c r="AB12">
-        <v>538.3503600000001</v>
+        <v>688.6417200000001</v>
       </c>
       <c r="AC12">
-        <v>415.12621</v>
+        <v>445.20755</v>
       </c>
       <c r="AD12">
-        <v>459.07326</v>
+        <v>620.2553599999999</v>
       </c>
       <c r="AE12">
-        <v>320.26875</v>
+        <v>400.86309</v>
       </c>
       <c r="AF12">
-        <v>432876.743</v>
+        <v>3715969.31</v>
       </c>
       <c r="AG12">
         <v>10</v>
@@ -1690,94 +1690,94 @@
         <v>80</v>
       </c>
       <c r="C13">
-        <v>412689420</v>
+        <v>2721836400</v>
       </c>
       <c r="D13">
-        <v>2773291.13</v>
+        <v>379628800</v>
       </c>
       <c r="E13">
-        <v>7261.2841</v>
+        <v>8746.1587</v>
       </c>
       <c r="F13">
-        <v>45.857477</v>
+        <v>179.066669</v>
       </c>
       <c r="G13">
-        <v>35.898689</v>
+        <v>68.853318</v>
       </c>
       <c r="H13">
-        <v>15.803622</v>
+        <v>32.963964</v>
       </c>
       <c r="I13">
-        <v>78.22327600000001</v>
+        <v>138.55297</v>
       </c>
       <c r="J13">
-        <v>38.413002</v>
+        <v>57.683497</v>
       </c>
       <c r="K13">
-        <v>226.2112</v>
+        <v>766.6399699999999</v>
       </c>
       <c r="L13">
-        <v>1046.66878</v>
+        <v>1401.815</v>
       </c>
       <c r="M13">
-        <v>97.990109</v>
+        <v>332.4292</v>
       </c>
       <c r="N13">
-        <v>10927982.9</v>
+        <v>46652465</v>
       </c>
       <c r="O13">
-        <v>174705.523</v>
+        <v>104581.154</v>
       </c>
       <c r="P13">
-        <v>673.8023599999999</v>
+        <v>330.900523</v>
       </c>
       <c r="Q13">
-        <v>1589.959989</v>
+        <v>1984.72584</v>
       </c>
       <c r="R13">
-        <v>144.991439</v>
+        <v>262.4089300000001</v>
       </c>
       <c r="S13">
-        <v>61.982065</v>
+        <v>119.227018</v>
       </c>
       <c r="T13">
-        <v>166640.5026</v>
+        <v>573548.4469999999</v>
       </c>
       <c r="U13">
-        <v>2418.37142</v>
+        <v>3374.502179999999</v>
       </c>
       <c r="V13">
-        <v>80.751915</v>
+        <v>118.452833</v>
       </c>
       <c r="W13">
-        <v>121.994379</v>
+        <v>139.75586</v>
       </c>
       <c r="X13">
-        <v>130.730373</v>
+        <v>245.52947</v>
       </c>
       <c r="Y13">
-        <v>348.82262</v>
+        <v>379.31119</v>
       </c>
       <c r="Z13">
-        <v>244.11539</v>
+        <v>289.67457</v>
       </c>
       <c r="AA13">
-        <v>462.1043</v>
+        <v>565.7984799999999</v>
       </c>
       <c r="AB13">
-        <v>513.59986</v>
+        <v>688.6417200000001</v>
       </c>
       <c r="AC13">
-        <v>415.12621</v>
+        <v>445.20755</v>
       </c>
       <c r="AD13">
-        <v>459.07326</v>
+        <v>620.2553599999999</v>
       </c>
       <c r="AE13">
-        <v>320.26875</v>
+        <v>395.5968</v>
       </c>
       <c r="AF13">
-        <v>367221.273</v>
+        <v>3715969.31</v>
       </c>
       <c r="AG13">
         <v>10</v>
@@ -1791,94 +1791,94 @@
         <v>90</v>
       </c>
       <c r="C14">
-        <v>412689420</v>
+        <v>2709679300</v>
       </c>
       <c r="D14">
-        <v>2723435.64</v>
+        <v>338798788</v>
       </c>
       <c r="E14">
-        <v>7138.208200000001</v>
+        <v>8329.7757</v>
       </c>
       <c r="F14">
-        <v>45.563572</v>
+        <v>179.066669</v>
       </c>
       <c r="G14">
-        <v>35.570168</v>
+        <v>68.853318</v>
       </c>
       <c r="H14">
-        <v>15.147427</v>
+        <v>32.542572</v>
       </c>
       <c r="I14">
-        <v>73.645138</v>
+        <v>138.55297</v>
       </c>
       <c r="J14">
-        <v>38.413002</v>
+        <v>57.683497</v>
       </c>
       <c r="K14">
-        <v>222.19782</v>
+        <v>766.6399699999999</v>
       </c>
       <c r="L14">
-        <v>1040.36368</v>
+        <v>1401.815</v>
       </c>
       <c r="M14">
-        <v>88.87092299999999</v>
+        <v>332.4292</v>
       </c>
       <c r="N14">
-        <v>9557292.9</v>
+        <v>41889330</v>
       </c>
       <c r="O14">
-        <v>174705.523</v>
+        <v>97507.726</v>
       </c>
       <c r="P14">
-        <v>611.82426</v>
+        <v>325.509383</v>
       </c>
       <c r="Q14">
-        <v>1373.020319</v>
+        <v>1984.72584</v>
       </c>
       <c r="R14">
-        <v>144.991439</v>
+        <v>255.34574</v>
       </c>
       <c r="S14">
-        <v>61.982065</v>
+        <v>119.227018</v>
       </c>
       <c r="T14">
-        <v>124717.7226</v>
+        <v>535388.9469999999</v>
       </c>
       <c r="U14">
-        <v>2273.88002</v>
+        <v>3264.705779999999</v>
       </c>
       <c r="V14">
-        <v>76.71373100000001</v>
+        <v>117.352073</v>
       </c>
       <c r="W14">
-        <v>121.994379</v>
+        <v>139.75586</v>
       </c>
       <c r="X14">
-        <v>130.730373</v>
+        <v>241.91256</v>
       </c>
       <c r="Y14">
-        <v>348.82262</v>
+        <v>379.31119</v>
       </c>
       <c r="Z14">
-        <v>239.37895</v>
+        <v>289.67457</v>
       </c>
       <c r="AA14">
-        <v>461.58124</v>
+        <v>565.7984799999999</v>
       </c>
       <c r="AB14">
-        <v>506.03347</v>
+        <v>688.6417200000001</v>
       </c>
       <c r="AC14">
-        <v>415.12621</v>
+        <v>443.9185100000001</v>
       </c>
       <c r="AD14">
-        <v>459.07326</v>
+        <v>619.14964</v>
       </c>
       <c r="AE14">
-        <v>318.59844</v>
+        <v>391.17145</v>
       </c>
       <c r="AF14">
-        <v>367221.273</v>
+        <v>3402270.11</v>
       </c>
       <c r="AG14">
         <v>10</v>
@@ -1892,94 +1892,94 @@
         <v>100</v>
       </c>
       <c r="C15">
-        <v>379428000</v>
+        <v>2683581400</v>
       </c>
       <c r="D15">
-        <v>2723435.64</v>
+        <v>338798788</v>
       </c>
       <c r="E15">
-        <v>6928.633</v>
+        <v>8329.7757</v>
       </c>
       <c r="F15">
-        <v>41.826762</v>
+        <v>179.066669</v>
       </c>
       <c r="G15">
-        <v>33.728517</v>
+        <v>68.853318</v>
       </c>
       <c r="H15">
-        <v>14.559545</v>
+        <v>32.542572</v>
       </c>
       <c r="I15">
-        <v>71.33912300000001</v>
+        <v>137.1995</v>
       </c>
       <c r="J15">
-        <v>38.38777900000001</v>
+        <v>57.683497</v>
       </c>
       <c r="K15">
-        <v>219.33731</v>
+        <v>759.84132</v>
       </c>
       <c r="L15">
-        <v>1010.64768</v>
+        <v>1401.815</v>
       </c>
       <c r="M15">
-        <v>85.43773099999999</v>
+        <v>319.08114</v>
       </c>
       <c r="N15">
-        <v>9388733.800000001</v>
+        <v>41889330</v>
       </c>
       <c r="O15">
-        <v>138516.8</v>
+        <v>97507.726</v>
       </c>
       <c r="P15">
-        <v>611.82426</v>
+        <v>271.901863</v>
       </c>
       <c r="Q15">
-        <v>1070.644829</v>
+        <v>1984.72584</v>
       </c>
       <c r="R15">
-        <v>139.91504</v>
+        <v>233.07129</v>
       </c>
       <c r="S15">
-        <v>61.982065</v>
+        <v>112.128708</v>
       </c>
       <c r="T15">
-        <v>124717.7226</v>
+        <v>366152.637</v>
       </c>
       <c r="U15">
-        <v>1469.23992</v>
+        <v>3264.705779999999</v>
       </c>
       <c r="V15">
-        <v>73.53571700000001</v>
+        <v>112.727933</v>
       </c>
       <c r="W15">
-        <v>121.994379</v>
+        <v>137.86664</v>
       </c>
       <c r="X15">
-        <v>129.983723</v>
+        <v>241.91256</v>
       </c>
       <c r="Y15">
-        <v>347.04276</v>
+        <v>379.08742</v>
       </c>
       <c r="Z15">
-        <v>239.37895</v>
+        <v>288.42762</v>
       </c>
       <c r="AA15">
-        <v>461.01667</v>
+        <v>565.7984799999999</v>
       </c>
       <c r="AB15">
-        <v>506.03347</v>
+        <v>683.73543</v>
       </c>
       <c r="AC15">
-        <v>413.80386</v>
+        <v>443.9185100000001</v>
       </c>
       <c r="AD15">
-        <v>457.37676</v>
+        <v>619.14964</v>
       </c>
       <c r="AE15">
-        <v>315.7482200000001</v>
+        <v>389.1822</v>
       </c>
       <c r="AF15">
-        <v>331336.535</v>
+        <v>3402270.11</v>
       </c>
       <c r="AG15">
         <v>10</v>

</xml_diff>